<commit_message>
2024-07-10 23:22 Created basic view page"
</commit_message>
<xml_diff>
--- a/20240709-칼럼너비.xlsx
+++ b/20240709-칼럼너비.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ceoba\Dropbox\pjt\spring\js-document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{123EB8F5-94F1-4340-BC30-9F59E715B7A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15DE7EB5-6B2C-48F8-B74E-3D64CE726B48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0072B3B3-C95D-4453-B942-817BCC0EC635}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>분석 공동조사서</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -168,7 +168,19 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>그림4</t>
+    <t>평단면</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>공동단면</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>노면</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>실제 높이</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -176,6 +188,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="177" formatCode="0.0%"/>
+  </numFmts>
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -216,12 +231,18 @@
       <charset val="129"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -248,13 +269,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -592,10 +613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8733FAF-52D9-4D01-990D-291197E6FFC8}">
-  <dimension ref="B2:P21"/>
+  <dimension ref="B2:P39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999"/>
@@ -615,157 +636,111 @@
       </c>
     </row>
     <row r="3" spans="2:16">
+      <c r="B3" s="1">
+        <v>266.06</v>
+      </c>
+      <c r="M3" s="1">
+        <f>SUM(B3:L3)</f>
+        <v>266.06</v>
+      </c>
       <c r="O3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="P3" s="1">
-        <v>266.05</v>
+        <v>266.06</v>
       </c>
     </row>
     <row r="4" spans="2:16">
-      <c r="B4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="1">
-        <v>37.816955</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I4" s="1">
-        <v>53</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>10</v>
+      <c r="B4" s="1">
+        <v>11.4</v>
+      </c>
+      <c r="M4" s="4">
+        <v>11.4</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>13</v>
       </c>
       <c r="P4" s="1">
-        <v>162.07</v>
-      </c>
-    </row>
-    <row r="5" spans="2:16">
-      <c r="B5" s="1">
-        <v>22.86</v>
-      </c>
-      <c r="C5" s="1">
-        <v>82.88</v>
-      </c>
-      <c r="D5" s="1">
-        <v>8.32</v>
-      </c>
-      <c r="E5" s="1">
-        <v>8.32</v>
-      </c>
-      <c r="F5" s="1">
-        <v>46.97</v>
-      </c>
-      <c r="G5" s="1">
-        <v>8.56</v>
-      </c>
-      <c r="H5" s="1">
-        <v>30.46</v>
-      </c>
-      <c r="I5" s="1">
-        <v>12.35</v>
-      </c>
-      <c r="J5" s="1">
-        <v>8.86</v>
-      </c>
-      <c r="K5" s="1">
-        <v>8.86</v>
-      </c>
-      <c r="L5" s="1">
-        <v>27.62</v>
-      </c>
-      <c r="M5" s="1">
-        <f>SUM(B5:L5)</f>
-        <v>266.06</v>
+        <v>162.08000000000001</v>
       </c>
     </row>
     <row r="6" spans="2:16">
-      <c r="B6" s="2">
-        <f>B5/$P$3</f>
-        <v>8.5923698552903577E-2</v>
-      </c>
-      <c r="C6" s="2">
-        <f t="shared" ref="C6:L6" si="0">C5/$P$3</f>
-        <v>0.31152039090396538</v>
-      </c>
-      <c r="D6" s="2">
-        <f t="shared" si="0"/>
-        <v>3.1272317233602707E-2</v>
-      </c>
-      <c r="E6" s="2">
-        <f t="shared" si="0"/>
-        <v>3.1272317233602707E-2</v>
-      </c>
-      <c r="F6" s="2">
-        <f t="shared" si="0"/>
-        <v>0.17654576207479797</v>
-      </c>
-      <c r="G6" s="2">
-        <f t="shared" si="0"/>
-        <v>3.2174403307648938E-2</v>
-      </c>
-      <c r="H6" s="2">
-        <f t="shared" si="0"/>
-        <v>0.11448975756436759</v>
-      </c>
-      <c r="I6" s="2">
-        <f t="shared" si="0"/>
-        <v>4.6419845893629012E-2</v>
-      </c>
-      <c r="J6" s="2">
-        <f t="shared" si="0"/>
-        <v>3.3302010900206722E-2</v>
-      </c>
-      <c r="K6" s="2">
-        <f t="shared" si="0"/>
-        <v>3.3302010900206722E-2</v>
-      </c>
-      <c r="L6" s="2">
-        <f t="shared" si="0"/>
-        <v>0.10381507235482053</v>
-      </c>
-      <c r="M6" s="3">
-        <f>SUM(B6:L6)</f>
-        <v>1.0000375869197518</v>
+      <c r="O6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P6" s="1">
+        <f>SUM(M4,M9,M14,M19,M24,M34)</f>
+        <v>162.08000000000001</v>
       </c>
     </row>
     <row r="7" spans="2:16">
       <c r="B7" s="1" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="1">
+        <v>37.816955</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" s="1">
+        <v>53</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="2:16">
       <c r="B8" s="1">
-        <v>169.34</v>
+        <v>22.86</v>
       </c>
       <c r="C8" s="1">
-        <v>96.72</v>
+        <v>82.88</v>
+      </c>
+      <c r="D8" s="1">
+        <v>8.32</v>
+      </c>
+      <c r="E8" s="1">
+        <v>8.32</v>
+      </c>
+      <c r="F8" s="1">
+        <v>46.97</v>
+      </c>
+      <c r="G8" s="1">
+        <v>8.56</v>
+      </c>
+      <c r="H8" s="1">
+        <v>30.46</v>
+      </c>
+      <c r="I8" s="1">
+        <v>12.35</v>
+      </c>
+      <c r="J8" s="1">
+        <v>8.86</v>
+      </c>
+      <c r="K8" s="1">
+        <v>8.86</v>
+      </c>
+      <c r="L8" s="1">
+        <v>27.62</v>
       </c>
       <c r="M8" s="1">
         <f>SUM(B8:L8)</f>
@@ -773,194 +748,421 @@
       </c>
     </row>
     <row r="9" spans="2:16">
-      <c r="B9" s="2">
+      <c r="B9" s="1">
+        <v>6.95</v>
+      </c>
+      <c r="C9" s="1">
+        <v>6.95</v>
+      </c>
+      <c r="D9" s="1">
+        <v>27.8</v>
+      </c>
+      <c r="E9" s="1">
+        <v>6.95</v>
+      </c>
+      <c r="F9" s="1">
+        <v>6.95</v>
+      </c>
+      <c r="G9" s="1">
+        <v>27.8</v>
+      </c>
+      <c r="H9" s="1">
+        <v>6.95</v>
+      </c>
+      <c r="I9" s="1">
+        <v>6.95</v>
+      </c>
+      <c r="J9" s="1">
+        <v>13.9</v>
+      </c>
+      <c r="K9" s="1">
+        <v>6.95</v>
+      </c>
+      <c r="L9" s="1">
+        <v>6.95</v>
+      </c>
+      <c r="M9" s="4">
+        <f>6.95*4</f>
+        <v>27.8</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16">
+      <c r="B10" s="3">
         <f>B8/$P$3</f>
-        <v>0.63649689907912044</v>
-      </c>
-      <c r="C9" s="2">
-        <f>C8/$P$3</f>
-        <v>0.36354068784063143</v>
-      </c>
-      <c r="M9" s="3">
-        <f>SUM(B9:L9)</f>
-        <v>1.0000375869197518</v>
-      </c>
-    </row>
-    <row r="10" spans="2:16">
-      <c r="B10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>18</v>
+        <v>8.5920469067127719E-2</v>
+      </c>
+      <c r="C10" s="3">
+        <f t="shared" ref="C10:L10" si="0">C8/$P$3</f>
+        <v>0.31150868225212358</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" si="0"/>
+        <v>3.1271141847703528E-2</v>
+      </c>
+      <c r="E10" s="3">
+        <f t="shared" si="0"/>
+        <v>3.1271141847703528E-2</v>
+      </c>
+      <c r="F10" s="3">
+        <f t="shared" si="0"/>
+        <v>0.17653912651281664</v>
+      </c>
+      <c r="G10" s="3">
+        <f t="shared" si="0"/>
+        <v>3.2173194016387283E-2</v>
+      </c>
+      <c r="H10" s="3">
+        <f t="shared" si="0"/>
+        <v>0.11448545440877998</v>
+      </c>
+      <c r="I10" s="3">
+        <f t="shared" si="0"/>
+        <v>4.6418101180184919E-2</v>
+      </c>
+      <c r="J10" s="3">
+        <f t="shared" si="0"/>
+        <v>3.3300759227241974E-2</v>
+      </c>
+      <c r="K10" s="3">
+        <f t="shared" si="0"/>
+        <v>3.3300759227241974E-2</v>
+      </c>
+      <c r="L10" s="3">
+        <f t="shared" si="0"/>
+        <v>0.10381117041268886</v>
+      </c>
+      <c r="M10" s="2">
+        <f>SUM(B10:L10)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="2:16">
-      <c r="B11" s="1">
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="2"/>
+    </row>
+    <row r="12" spans="2:16">
+      <c r="B12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16">
+      <c r="B13" s="1">
         <v>169.34</v>
       </c>
-      <c r="C11" s="1">
-        <v>48.36</v>
-      </c>
-      <c r="D11" s="1">
-        <v>48.36</v>
-      </c>
-      <c r="M11" s="1">
-        <f>SUM(B11:L11)</f>
+      <c r="C13" s="1">
+        <v>96.72</v>
+      </c>
+      <c r="M13" s="1">
+        <f>SUM(B13:L13)</f>
         <v>266.06</v>
-      </c>
-    </row>
-    <row r="12" spans="2:16">
-      <c r="B12" s="2">
-        <f>B11/$P$3</f>
-        <v>0.63649689907912044</v>
-      </c>
-      <c r="C12" s="2">
-        <f>C11/$P$3</f>
-        <v>0.18177034392031571</v>
-      </c>
-      <c r="D12" s="2">
-        <f>D11/$P$3</f>
-        <v>0.18177034392031571</v>
-      </c>
-      <c r="M12" s="3">
-        <f>SUM(B12:L12)</f>
-        <v>1.000037586919752</v>
-      </c>
-    </row>
-    <row r="13" spans="2:16">
-      <c r="B13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="14" spans="2:16">
       <c r="B14" s="1">
+        <v>7.34</v>
+      </c>
+      <c r="C14" s="1">
+        <v>7.34</v>
+      </c>
+      <c r="M14" s="4">
+        <v>7.34</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16">
+      <c r="B15" s="3">
+        <f>B13/$P$3</f>
+        <v>0.6364729760204465</v>
+      </c>
+      <c r="C15" s="3">
+        <f>C13/$P$3</f>
+        <v>0.3635270239795535</v>
+      </c>
+      <c r="M15" s="2">
+        <f>SUM(B15:L15)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16">
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="M16" s="2"/>
+    </row>
+    <row r="17" spans="2:13">
+      <c r="B17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13">
+      <c r="B18" s="1">
+        <v>169.34</v>
+      </c>
+      <c r="C18" s="1">
+        <v>48.36</v>
+      </c>
+      <c r="D18" s="1">
+        <v>48.36</v>
+      </c>
+      <c r="M18" s="1">
+        <f>SUM(B18:L18)</f>
+        <v>266.06</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13">
+      <c r="B19" s="1">
+        <v>57.08</v>
+      </c>
+      <c r="C19" s="1">
+        <v>28.54</v>
+      </c>
+      <c r="D19" s="1">
+        <v>28.54</v>
+      </c>
+      <c r="M19" s="4">
+        <v>57.08</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13">
+      <c r="B20" s="3">
+        <f>B18/$P$3</f>
+        <v>0.6364729760204465</v>
+      </c>
+      <c r="C20" s="3">
+        <f>C18/$P$3</f>
+        <v>0.18176351198977675</v>
+      </c>
+      <c r="D20" s="3">
+        <f>D18/$P$3</f>
+        <v>0.18176351198977675</v>
+      </c>
+      <c r="M20" s="2">
+        <f>SUM(B20:L20)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13">
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="M21" s="2"/>
+    </row>
+    <row r="22" spans="2:13">
+      <c r="B22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13">
+      <c r="B23" s="1">
         <v>131.28</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C23" s="1">
         <v>85.12</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D23" s="1">
         <v>49.66</v>
       </c>
-      <c r="M14" s="1">
-        <f>SUM(B14:L14)</f>
+      <c r="M23" s="1">
+        <f>SUM(B23:L23)</f>
         <v>266.06</v>
       </c>
     </row>
-    <row r="15" spans="2:16">
-      <c r="B15" s="2">
-        <f>B14/$P$3</f>
-        <v>0.49344108250328883</v>
-      </c>
-      <c r="C15" s="2">
-        <f>C14/$P$3</f>
-        <v>0.31993986092839694</v>
-      </c>
-      <c r="D15" s="2">
-        <f>D14/$P$3</f>
-        <v>0.18665664348806613</v>
-      </c>
-      <c r="M15" s="3">
-        <f>SUM(B15:L15)</f>
-        <v>1.000037586919752</v>
-      </c>
-    </row>
-    <row r="16" spans="2:16">
-      <c r="C16" s="1" t="s">
+    <row r="24" spans="2:13">
+      <c r="B24" s="1">
+        <v>10.46</v>
+      </c>
+      <c r="C24" s="1">
+        <v>5.23</v>
+      </c>
+      <c r="D24" s="1">
+        <v>10.46</v>
+      </c>
+      <c r="M24" s="4">
+        <v>10.46</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13">
+      <c r="B25" s="3">
+        <f>B23/$P$3</f>
+        <v>0.49342253627001426</v>
+      </c>
+      <c r="C25" s="3">
+        <f>C23/$P$3</f>
+        <v>0.3199278358265053</v>
+      </c>
+      <c r="D25" s="3">
+        <f>D23/$P$3</f>
+        <v>0.18664962790348041</v>
+      </c>
+      <c r="M25" s="2">
+        <f>SUM(B25:L25)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13">
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="M26" s="2"/>
+    </row>
+    <row r="27" spans="2:13">
+      <c r="C27" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="2:13">
-      <c r="C17" s="1">
+    <row r="28" spans="2:13">
+      <c r="C28" s="1">
         <v>42.56</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D28" s="1">
         <v>42.56</v>
       </c>
-      <c r="M17" s="1">
-        <f>SUM(B17:L17)</f>
+      <c r="M28" s="1">
+        <f>SUM(B28:L28)</f>
         <v>85.12</v>
       </c>
     </row>
-    <row r="18" spans="2:13">
-      <c r="C18" s="2">
-        <f>C17/$P$3</f>
-        <v>0.15996993046419847</v>
-      </c>
-      <c r="D18" s="2">
-        <f>D17/$P$3</f>
-        <v>0.15996993046419847</v>
-      </c>
-      <c r="M18" s="3">
-        <f>SUM(B18:L18)</f>
-        <v>0.31993986092839694</v>
-      </c>
-    </row>
-    <row r="19" spans="2:13">
-      <c r="B19" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E19" s="1" t="s">
+    <row r="29" spans="2:13">
+      <c r="C29" s="1">
+        <v>5.23</v>
+      </c>
+      <c r="D29" s="1">
+        <v>5.23</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13">
+      <c r="C30" s="3">
+        <f>C28/$P$3</f>
+        <v>0.15996391791325265</v>
+      </c>
+      <c r="D30" s="3">
+        <f>D28/$P$3</f>
+        <v>0.15996391791325265</v>
+      </c>
+      <c r="M30" s="2">
+        <f>SUM(B30:L30)</f>
+        <v>0.3199278358265053</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13">
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="M31" s="2"/>
+    </row>
+    <row r="32" spans="2:13">
+      <c r="B32" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="M19" s="4"/>
-    </row>
-    <row r="20" spans="2:13">
-      <c r="B20" s="1">
+      <c r="C32" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="2:13">
+      <c r="B33" s="1">
         <v>131.28</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C33" s="1">
         <v>42.56</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D33" s="1">
         <v>42.56</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E33" s="1">
         <v>49.66</v>
       </c>
-      <c r="M20" s="1">
-        <f>SUM(B20:L20)</f>
+      <c r="M33" s="1">
+        <f>SUM(B33:L33)</f>
         <v>266.06</v>
       </c>
     </row>
-    <row r="21" spans="2:13">
-      <c r="B21" s="2">
-        <f>B20/$P$3</f>
-        <v>0.49344108250328883</v>
-      </c>
-      <c r="C21" s="2">
-        <f>C20/$P$3</f>
-        <v>0.15996993046419847</v>
-      </c>
-      <c r="D21" s="2">
-        <f>D20/$P$3</f>
-        <v>0.15996993046419847</v>
-      </c>
-      <c r="E21" s="2">
-        <f>E20/$P$3</f>
-        <v>0.18665664348806613</v>
-      </c>
-      <c r="M21" s="3">
-        <f>SUM(B21:L21)</f>
-        <v>1.000037586919752</v>
+    <row r="34" spans="2:13">
+      <c r="B34" s="1">
+        <v>15</v>
+      </c>
+      <c r="C34" s="1">
+        <v>48</v>
+      </c>
+      <c r="D34" s="1">
+        <v>48</v>
+      </c>
+      <c r="E34" s="1">
+        <v>48</v>
+      </c>
+      <c r="M34" s="4">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" spans="2:13">
+      <c r="B35" s="3">
+        <f>B33/$P$3</f>
+        <v>0.49342253627001426</v>
+      </c>
+      <c r="C35" s="3">
+        <f>C33/$P$3</f>
+        <v>0.15996391791325265</v>
+      </c>
+      <c r="D35" s="3">
+        <f>D33/$P$3</f>
+        <v>0.15996391791325265</v>
+      </c>
+      <c r="E35" s="3">
+        <f>E33/$P$3</f>
+        <v>0.18664962790348041</v>
+      </c>
+      <c r="M35" s="2">
+        <f>SUM(B35:L35)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="2:13">
+      <c r="B37" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" spans="2:13">
+      <c r="B38" s="1">
+        <v>131.28</v>
+      </c>
+      <c r="M38" s="1">
+        <f>SUM(B38:L38)</f>
+        <v>131.28</v>
+      </c>
+    </row>
+    <row r="39" spans="2:13">
+      <c r="B39" s="1">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>